<commit_message>
refactor: Update QuotationController store method to include session ID and send additional email for quotations
</commit_message>
<xml_diff>
--- a/storage/app/import/meta_data.xlsx
+++ b/storage/app/import/meta_data.xlsx
@@ -328,7 +328,7 @@
     <t>Aero, tolóajtó, Loft stílus, fekete fém sín, indusztriális karakter, egyszárnyú változat, süllyesztett acél fogantyú, kollekciók, csomagolás.</t>
   </si>
   <si>
-    <t>MODI DESIGN tolóajtó rendszer</t>
+    <t>Modi Design sliding system</t>
   </si>
   <si>
     <t>A MODI system egy modern tolóajtócsalád, ideális választás Loft stílusú lakásokba. A fekete fém sín, görgő és kiegészítő elemek indusztriális jellegűvé teszik az ajtót. A rendszer közvetlenül falra szerelhető, csak egyszárnyú változatban érhető el. Az ajtószárnyak magassága 2035 mm, és elérhetők 70', 80', 90' szélességben, fekete süllyesztett acél fogantyúval. Az ajtókat külön kell megvásárolni, és minden kollekcióban és dekorban elérhetők, kivéve: Classic, Andromeda, Salvano. A csomag tartalmazza a komplett tolóajtó rendszert 1950 mm hosszú sínnel. Zárható kivitel is rendelhető felár ellenében.</t>
@@ -337,7 +337,7 @@
     <t>MODI system, tolóajtó, Loft stílus, fekete fém sín, indusztriális karakter, egyszárnyú változat, süllyesztett acél fogantyú, kollekciók, csomagolás.</t>
   </si>
   <si>
-    <t>Egy és kétszárnyú tolóajtó rendszerek</t>
+    <t>Single leaf and double leaf sliding system</t>
   </si>
   <si>
     <t>Az egyszárnyú fal előtti csúszó rendszer lehetővé teszi az egyszárnyú tolóajtókat falra szerelt karnissal és ajtóütközővel. Rendelhető különböző méretekben: 60', 70', 80', 90', 100'. Tartalmazza a takarólécet ajtóütközővel, egyszárnyú ajtólapot és tolóajtó sínt. A kétszárnyú fal előtti csúszó rendszer szinkronban nyitható, két azonos szélességű ajtólapot igényel, melyeket egyidejűleg lehet nyitni egy szárny elcsúsztatásával. Kapható különböző méretekben: 120', 140', 160', 180', 200'. Tartalmazza a szinkron csúszó elemet/vasalatot, takarólécet és kétszárnyú kivitelt. A csúszórendszer elérhető minden dekorban és kollekcióban, kivéve a Classic, Andromeda, Salvano és Ksantos New kollekciókat.</t>
@@ -355,7 +355,7 @@
     <t>falcolt ajtólap, becsavarható pánt, kulcsos zár, wc, biztonsági zár, átjáró zár, blokk ajtótok, állítható ajtótok, értesítés, zsanér, dekor, Acacia ST, Natural Oak, Riviera Oak, Burnt Oak, Wenge, Gray Matt, perforált forgácslap, lágyfa keret.</t>
   </si>
   <si>
-    <t>Állítható falcolt tok</t>
+    <t>Adjustable door frame</t>
   </si>
   <si>
     <t>Az állítható ajtótokok faforgácslapból és MDF-ből készülnek, Classen Primo, Classen 3D look, Classen Iridium fólia és Classen CPL laminátum bevonattal, mindig az ajtólap dekoroknak megfelelő felületi minőségben. Átjáró tok változatban is elérhető. A komplett ajtótok tartalmazza a felső összekötő és a két függőleges álló elemet, valamint a gumitömítést és az összeszereléshez szükséges segédanyagokat. A 110’ méretű vagy megerősített szerkezetű ajtószárnyakhoz három zsanéros ajtótok szükséges. A színpaletta tartalmazza a Classen Primo, Classen 3D Prémium dekor, Classen Iridium és Classen CPL dekorokat, valamint lakkozott és RAL színeket is, melyek feláras lehetőségek. Az állítható tokok 80 mm szélességű takaróléccel is rendelhetőek, kivéve a Natura HK CPL - PN22 és PN23 modelleknél.</t>
@@ -364,7 +364,7 @@
     <t>állítható ajtótok, faforgácslap, MDF, Classen Primo, Classen 3D look, Classen Iridium, Classen CPL, dekor, laminátum, fólia, átjáró tok, felső összekötő, függőleges álló elem, gumitömítés, összeszerelés, zsanér, színpaletta, lakkozott, RAL színek, takaróléc.</t>
   </si>
   <si>
-    <t>Állítható falcolatlan tok</t>
+    <t>Adjustable non-rebated door frame</t>
   </si>
   <si>
     <t>Az állítható falcolatlan ajtótokok MDF-ből és forgácslapból készülnek, Classen dekorral borítják, vagy ajtólap felületének megfelelő színű lakkozással felületkezzelik. Az ajtótok az ajtólapokkal megegyező laminátummal vagy festéssel készül. A falcolatlan "B" ajtólapokhoz megfelelő. A komplett, falcolatlan ajtótok felső összekötőből és függőleges álló tokelemből áll, és egy csomagot alkot. A készlet tartalmaz két speciális 3D pántot, gumitömítést és egy szerelőcsomagot.</t>
@@ -373,7 +373,7 @@
     <t>állítható ajtótok, falcolatlan, MDF, forgácslap, Classen dekor, lakkozás, laminátum, festés, 3D pánt, gumitömítés, szerelőcsomag, színpaletta, RAL színek, takaróléc.</t>
   </si>
   <si>
-    <t>Blokk tok</t>
+    <t>Standard 2-Pack door frame</t>
   </si>
   <si>
     <t>A Blokk ajtótokok MDF-ből készülnek, laminált felülettel, az ajtólap dekoroknak megfelelő dekor választékban. Átjáró tok változatban is elérhetőek. A teljes ajtótok a felső összekötőelemmel és két függőleges álló elemmel áll, amelyek két külön csomagban érkeznek, és két nikkelezett pánttal vannak felszerelve (a harmadik zsanér felár ellenében rendelhető). Három zsanéros ajtótokot kell használni 110' méretű vagy megerősített ajtószárnyak esetén.</t>
@@ -413,11 +413,14 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -634,8 +637,8 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.38"/>
-    <col customWidth="1" min="2" max="2" width="18.75"/>
+    <col customWidth="1" min="1" max="1" width="37.13"/>
+    <col customWidth="1" min="2" max="2" width="30.25"/>
     <col customWidth="1" min="3" max="3" width="18.88"/>
   </cols>
   <sheetData>
@@ -1036,7 +1039,7 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>105</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -1047,7 +1050,7 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>108</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -1069,7 +1072,7 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>114</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -1080,7 +1083,7 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>117</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -1091,7 +1094,7 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>120</v>
       </c>
       <c r="B42" s="1" t="s">

</xml_diff>